<commit_message>
i make update in backend
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,321 +440,529 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>price</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>discount</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>amount</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>category</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>price</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>discount</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>created_at</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>finalPrice</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>image</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>category</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>amount</t>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>updated_at</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>ratings</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>average_rating</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>images</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>67c5e4b28a712a7d8772e3b8</t>
+          <t>clock 22</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>rice</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>200</v>
-      </c>
-      <c r="D2" t="n">
-        <v>20</v>
-      </c>
-      <c r="E2" t="n">
-        <v>160</v>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>good</t>
+        </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>/static/img/uploads/images.jpg</t>
+          <t>watches</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>sooooo goood</t>
+          <t>/static/img/uploads/watches3.jpg</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>shoes</t>
-        </is>
-      </c>
-      <c r="I2" t="n">
-        <v>1</v>
-      </c>
+          <t>67e2a770015b0d98f2e9ac84</t>
+        </is>
+      </c>
+      <c r="I2" s="2" t="n">
+        <v>45741.53760061342</v>
+      </c>
+      <c r="J2" t="n">
+        <v>240</v>
+      </c>
+      <c r="K2" s="2" t="n">
+        <v>45742.75040645833</v>
+      </c>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>67c5e4e38a712a7d8772e3ba</t>
+          <t>shose2</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>oil</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>50</v>
+          <t>800</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>70</t>
+        </is>
       </c>
       <c r="D3" t="n">
-        <v>10</v>
-      </c>
-      <c r="E3" t="n">
-        <v>45</v>
+        <v>51</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>sport</t>
+        </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>/static/img/uploads/77.jpg</t>
+          <t>shoes</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>soooogooood</t>
+          <t>/static/img/uploads/shoes3.jpg</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>clothing</t>
-        </is>
-      </c>
-      <c r="I3" t="n">
-        <v>1</v>
-      </c>
+          <t>67e2a83e015b0d98f2e9ac8c</t>
+        </is>
+      </c>
+      <c r="I3" s="2" t="n">
+        <v>45741.53998518518</v>
+      </c>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>[{'user': 'Kar', 'rating': 5, 'comment': 'Soooooogooooood', 'date': datetime.datetime(2025, 3, 28, 21, 41, 7, 834000)}, {'user': 'Kar', 'rating': 5, 'comment': 'Soooooogooooood', 'date': datetime.datetime(2025, 3, 28, 21, 41, 8, 495000)}, {'user': 'Kar', 'rating': 5, 'comment': 'Soooooogooooood', 'date': datetime.datetime(2025, 3, 28, 21, 41, 9, 335000)}, {'user': 'Kar', 'rating': 5, 'comment': 'Soooooogooooood', 'date': datetime.datetime(2025, 3, 28, 21, 41, 9, 338000)}, {'user': 'admin', 'rating': 1, 'comment': 'واحد شنكلني ووقعت فعلا منكوا لله', 'date': datetime.datetime(2025, 3, 29, 11, 47, 51, 704000)}]</t>
+        </is>
+      </c>
+      <c r="M3" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="N3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>67c5e5218a712a7d8772e3bc</t>
+          <t>shose4</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>oil 3</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>600</v>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
       </c>
       <c r="D4" t="n">
-        <v>70</v>
-      </c>
-      <c r="E4" t="n">
-        <v>180</v>
+        <v>1</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>soo good</t>
+        </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>/static/img/uploads/png-clipart-olive-oil-liqueur-glass-bottle-vegetable-oil-olive-oil-glass-oil.png</t>
+          <t>shoes</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>bage goooood</t>
+          <t>/static/img/uploads/shoes1.jpg</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>clothing</t>
-        </is>
-      </c>
-      <c r="I4" t="n">
+          <t>67e2a87a015b0d98f2e9ac90</t>
+        </is>
+      </c>
+      <c r="I4" s="2" t="n">
+        <v>45741.54068256944</v>
+      </c>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>[{'user': 'mohamed', 'rating': 1, 'comment': ';knknknkl', 'date': datetime.datetime(2025, 3, 27, 20, 35, 45, 742000)}]</t>
+        </is>
+      </c>
+      <c r="M4" t="n">
         <v>1</v>
       </c>
+      <c r="N4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>67c5e5858a712a7d8772e3be</t>
+          <t>close 1</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>oil4</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>600</v>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
       </c>
       <c r="D5" t="n">
-        <v>30</v>
-      </c>
-      <c r="E5" t="n">
-        <v>420</v>
+        <v>27</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">soo good </t>
+        </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>/static/img/uploads/OIP.jpg</t>
+          <t>clothing</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>soooooo goooood</t>
+          <t>/static/img/uploads/clothes3.jpg</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>clothing</t>
-        </is>
-      </c>
-      <c r="I5" t="n">
-        <v>1</v>
-      </c>
+          <t>67e2a8ea015b0d98f2e9ac92</t>
+        </is>
+      </c>
+      <c r="I5" s="2" t="n">
+        <v>45741.54197435185</v>
+      </c>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>67c5e6cc8a712a7d8772e3c0</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>rice2</t>
-        </is>
+          <t xml:space="preserve"> closes</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>100</v>
       </c>
       <c r="C6" t="n">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>10</v>
-      </c>
-      <c r="E6" t="n">
-        <v>180</v>
+        <v>1</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>adcac</t>
+        </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>/static/img/uploads/images.jpg</t>
+          <t>clothing</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>sooo goood</t>
+          <t>/static/img/uploads/clothes4.jpg</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>shoes</t>
-        </is>
-      </c>
-      <c r="I6" t="n">
-        <v>1</v>
+          <t>67e7dc8002f5a732f4dd8e4b</t>
+        </is>
+      </c>
+      <c r="I6" s="2" t="n">
+        <v>45745.48740796297</v>
+      </c>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>['/static/img/uploads/clothes.jpg']</t>
+        </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>67c5e70f8a712a7d8772e3c2</t>
+          <t xml:space="preserve"> closes</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>rice 3</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>300</v>
-      </c>
-      <c r="D7" t="n">
-        <v>50</v>
-      </c>
-      <c r="E7" t="n">
-        <v>150</v>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>cdddcddc</t>
+        </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>/static/img/uploads/th.jpg</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>soooooogooooood</t>
-        </is>
-      </c>
+          <t>clothing</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr">
         <is>
-          <t>shoes</t>
-        </is>
-      </c>
-      <c r="I7" t="n">
-        <v>1</v>
+          <t>67e7dccfb78ff53ca5b59e61</t>
+        </is>
+      </c>
+      <c r="I7" s="2" t="n">
+        <v>45745.48833255787</v>
+      </c>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>['/static/img/uploads/clothes1.jpg']</t>
+        </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>67c5e75b8a712a7d8772e3c4</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>rice3</t>
-        </is>
+          <t xml:space="preserve"> closes200</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>100</v>
       </c>
       <c r="C8" t="n">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="D8" t="n">
-        <v>10</v>
-      </c>
-      <c r="E8" t="n">
-        <v>90</v>
+        <v>3</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>sooo</t>
+        </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>/static/img/uploads/th (1).jpg</t>
+          <t>clothing</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>soooooooogooooooooood</t>
+          <t>/static/img/uploads/clothes1.jpg</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>shoes</t>
-        </is>
-      </c>
-      <c r="I8" t="n">
-        <v>1</v>
+          <t>67e7e00db78ff53ca5b59e63</t>
+        </is>
+      </c>
+      <c r="I8" s="2" t="n">
+        <v>45745.49792914352</v>
+      </c>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> closes500</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2000</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>70</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>cacadad</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>clothing</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>67e7e276b78ff53ca5b59e65</t>
+        </is>
+      </c>
+      <c r="I9" s="2" t="n">
+        <v>45745.50507430555</v>
+      </c>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> closes500</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>2000</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>70</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>cacadad</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>clothing</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>67e7e2a8b78ff53ca5b59e67</t>
+        </is>
+      </c>
+      <c r="I10" s="2" t="n">
+        <v>45745.50565765046</v>
+      </c>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>